<commit_message>
- [x] Password generated and excel stored - [x] Project completed
</commit_message>
<xml_diff>
--- a/NewJoiners.xlsx
+++ b/NewJoiners.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianca.dragu\Documents\UiPath\NewJoinerPasswords\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tolnaib\Documents\Learn to Program\UiPath\Password generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75E0D46-271D-4B5F-965E-50AA1C1C877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
   </bookViews>
   <sheets>
     <sheet name="NewJoiners" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>first_name</t>
   </si>
@@ -140,12 +139,48 @@
   </si>
   <si>
     <t>inna.ofogarty@vitaminui.com</t>
+  </si>
+  <si>
+    <t>PHBIwc4+^Kp9</t>
+  </si>
+  <si>
+    <t>&gt;m&lt;Ot42gtk$M</t>
+  </si>
+  <si>
+    <t>2A#(%46dc4y)</t>
+  </si>
+  <si>
+    <t>i26G1ji51*cl</t>
+  </si>
+  <si>
+    <t>i12#!-(()+&lt;4</t>
+  </si>
+  <si>
+    <t>NJ3909O+*6&lt;P</t>
+  </si>
+  <si>
+    <t>^3^&lt;sCo2&amp;#HJ</t>
+  </si>
+  <si>
+    <t>IEa+%tB@(J23</t>
+  </si>
+  <si>
+    <t>3(^@K%#GdgP&amp;</t>
+  </si>
+  <si>
+    <t>B^+8$q%+d#J%</t>
+  </si>
+  <si>
+    <t>5f$dB8!cnJE&gt;</t>
+  </si>
+  <si>
+    <t>cEF4NN+^52d3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -979,7 +1014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1012,6 +1047,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1023,6 +1061,9 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1034,6 +1075,9 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1045,6 +1089,9 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1056,6 +1103,9 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1067,6 +1117,9 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1078,6 +1131,9 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1089,6 +1145,9 @@
       <c r="C9" t="s">
         <v>27</v>
       </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1100,6 +1159,9 @@
       <c r="C10" t="s">
         <v>30</v>
       </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1111,6 +1173,9 @@
       <c r="C11" t="s">
         <v>33</v>
       </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1122,6 +1187,9 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1132,6 +1200,9 @@
       </c>
       <c r="C13" t="s">
         <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>